<commit_message>
Fix cargo-dist conversion factor in webtool
</commit_message>
<xml_diff>
--- a/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
+++ b/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\web-app\CDCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\web-app\CDCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D18836A-B39E-44FA-BBD8-FA20656F100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD1AAA1-F480-44F3-8E00-464726421EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="960" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30195" yWindow="2895" windowWidth="25590" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -449,27 +449,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,53 +477,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>1.60934</v>
+        <v>0.62136999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -543,24 +543,24 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <f>10^12*About!B16</f>
-        <v>1609340000000</v>
+        <v>621370000000</v>
       </c>
     </row>
   </sheetData>
@@ -575,28 +575,28 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
         <f>10^12*About!B16</f>
-        <v>1609340000000</v>
+        <v>621370000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>